<commit_message>
Added options to view manual and COE papers from Asmita Help menu Corrected Southampton exercise to make changes in 2020 and 2030 and to include answers for cases with and without the maintenance dredging.
git-svn-id: svn://192.168.0.80/muiApps/Trunk/Asmita@164 5305ae0c-0cd9-424f-b575-fb45b188e99a
</commit_message>
<xml_diff>
--- a/Training exercise/Training exercise-Southampton/SW4e_results.xlsx
+++ b/Training exercise/Training exercise-Southampton/SW4e_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab Code\MUImodels\muiApps\Asmita\Training exercise\Training exercise-Southampton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989B3109-72EC-4114-BF0F-4F64A8EBF9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D78646B-27D2-4378-BD7D-C006A428DFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7300" yWindow="4080" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9940" yWindow="2180" windowWidth="21940" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Year</t>
   </si>
@@ -57,9 +57,6 @@
     <t>+area change =</t>
   </si>
   <si>
-    <t>Results using v1.4</t>
-  </si>
-  <si>
     <t>SW4e model - Case (excl maintenance)</t>
   </si>
   <si>
@@ -75,16 +72,31 @@
     <t>3 – historic changes + slr</t>
   </si>
   <si>
-    <t>4 – As 3, with dredge in 2000*</t>
-  </si>
-  <si>
-    <t>5 – As 4, with reclamation in 2020*</t>
-  </si>
-  <si>
     <t>% change from</t>
   </si>
   <si>
     <t>1900 volume</t>
+  </si>
+  <si>
+    <t>Results using v3.1</t>
+  </si>
+  <si>
+    <t>Inner Channel</t>
+  </si>
+  <si>
+    <t>Outer Flat</t>
+  </si>
+  <si>
+    <t>Inner Flat</t>
+  </si>
+  <si>
+    <t>Outer Channel</t>
+  </si>
+  <si>
+    <t>4 – As 3, with dredge in 2020</t>
+  </si>
+  <si>
+    <t>5 – As 4, with reclamation in 2030</t>
   </si>
 </sst>
 </file>
@@ -490,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -509,7 +521,7 @@
     <col min="9" max="9" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -526,397 +538,493 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B3" s="5">
         <v>10000</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C3" s="5">
         <v>8000</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D3" s="5">
         <v>10000</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E3" s="5">
         <v>8000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>2020</v>
       </c>
-      <c r="B4" s="4">
-        <f>B2*200*2</f>
+      <c r="B5" s="4">
+        <f>B3*200*2</f>
         <v>4000000</v>
       </c>
-      <c r="C4" s="4">
-        <f>C2*200*2</f>
+      <c r="C5" s="4">
+        <f>C3*200*2</f>
         <v>3200000</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="4">
-        <f>B4+C4</f>
-        <v>7200000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2030</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
       </c>
       <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <f>B5+C5</f>
+        <v>7200000</v>
+      </c>
+      <c r="J5" s="4">
+        <f>C5+280000</f>
+        <v>3480000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2030</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
         <v>-500000</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G6" s="7">
         <v>-200000</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
         <v>1900</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C9" s="2">
         <v>2100</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="2">
         <v>1900</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G9" s="2">
         <v>2100</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4">
+      <c r="B11" s="4">
         <v>64011700</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C11" s="4">
         <v>64769700</v>
-      </c>
-      <c r="D10" s="4">
-        <f>C10-B10</f>
-        <v>758000</v>
-      </c>
-      <c r="E10" s="8">
-        <f>(D10)/B$10</f>
-        <v>1.1841585210203759E-2</v>
-      </c>
-      <c r="F10">
-        <v>57129700</v>
-      </c>
-      <c r="G10">
-        <v>44123700</v>
-      </c>
-      <c r="H10" s="4">
-        <f t="shared" ref="H10:H14" si="0">G10-F10</f>
-        <v>-13006000</v>
-      </c>
-      <c r="I10" s="8">
-        <f t="shared" ref="I10:I14" si="1">(H10)/F$10</f>
-        <v>-0.22765741812052226</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="4">
-        <v>65320700</v>
-      </c>
-      <c r="C11">
-        <v>66900400</v>
       </c>
       <c r="D11" s="4">
         <f>C11-B11</f>
+        <v>758000</v>
+      </c>
+      <c r="E11" s="8">
+        <f>(D11)/B$11</f>
+        <v>1.1841585210203759E-2</v>
+      </c>
+      <c r="F11">
+        <v>57129700</v>
+      </c>
+      <c r="G11">
+        <v>44123700</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" ref="H11:H15" si="0">G11-F11</f>
+        <v>-13006000</v>
+      </c>
+      <c r="I11" s="8">
+        <f t="shared" ref="I11:I15" si="1">(H11)/F$11</f>
+        <v>-0.22765741812052226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>65320700</v>
+      </c>
+      <c r="C12">
+        <v>66900400</v>
+      </c>
+      <c r="D12" s="4">
+        <f>C12-B12</f>
         <v>1579700</v>
       </c>
-      <c r="E11" s="8">
-        <f>(D11)/B$10</f>
+      <c r="E12" s="8">
+        <f>(D12)/B$11</f>
         <v>2.4678300998098784E-2</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <v>59209900</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G12" s="4">
         <v>46238000</v>
       </c>
-      <c r="H11" s="4">
-        <f>G11-F11</f>
+      <c r="H12" s="4">
+        <f>G12-F12</f>
         <v>-12971900</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I12" s="8">
         <f t="shared" si="1"/>
         <v>-0.22706053068719073</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
         <v>64011700</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C13" s="4">
         <v>72496900</v>
       </c>
-      <c r="D12" s="4">
-        <f t="shared" ref="D12:D14" si="2">C12-B12</f>
+      <c r="D13" s="4">
+        <f t="shared" ref="D13" si="2">C13-B13</f>
         <v>8485200</v>
       </c>
-      <c r="E12" s="8">
-        <f t="shared" ref="E12:E15" si="3">(D12)/B$10</f>
+      <c r="E13" s="8">
+        <f t="shared" ref="E13:E16" si="3">(D13)/B$11</f>
         <v>0.13255701692034424</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>57129700</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G13" s="4">
         <v>53119900</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H13" s="4">
         <f t="shared" si="0"/>
         <v>-4009800</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I13" s="8">
         <f t="shared" si="1"/>
         <v>-7.0187660708878219E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="4">
         <v>64011700</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C14" s="4">
         <v>74519500</v>
       </c>
-      <c r="D13" s="4">
-        <f>C13-B13</f>
+      <c r="D14" s="4">
+        <f>C14-B14</f>
         <v>10507800</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E14" s="8">
         <f t="shared" si="3"/>
         <v>0.16415436553005153</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>57129700</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G14" s="4">
         <v>55142400</v>
       </c>
-      <c r="H13" s="4">
-        <f>G13-F13</f>
+      <c r="H14" s="4">
+        <f>G14-F14</f>
         <v>-1987300</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I14" s="8">
         <f t="shared" si="1"/>
         <v>-3.4785759421106711E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4">
         <v>64011700</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C15" s="4">
         <v>74023300</v>
       </c>
-      <c r="D14" s="4">
-        <f>C14-B14</f>
+      <c r="D15" s="4">
+        <f>C15-B15</f>
         <v>10011600</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E15" s="8">
         <f t="shared" si="3"/>
         <v>0.15640265763915034</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>57129700</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G15" s="4">
         <v>54674700</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H15" s="4">
         <f t="shared" si="0"/>
         <v>-2455000</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I15" s="8">
         <f t="shared" si="1"/>
         <v>-4.2972394393809177E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="4">
-        <f>C14-C12</f>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="4">
+        <f>C15-C13</f>
         <v>1526400</v>
       </c>
-      <c r="D15" s="4">
-        <f>D13-D12</f>
+      <c r="D16" s="4">
+        <f>D14-D13</f>
         <v>2022600</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E16" s="8">
         <f t="shared" si="3"/>
         <v>3.1597348609707289E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="4">
-        <v>64011700</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17">
-        <v>57129700</v>
+    <row r="17" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B18" s="4">
         <v>64011700</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="C18" s="4">
+        <v>64769700</v>
+      </c>
+      <c r="D18" s="4">
+        <f>C18-B18</f>
+        <v>758000</v>
+      </c>
+      <c r="E18" s="8">
+        <f>(D18)/B$11</f>
+        <v>1.1841585210203759E-2</v>
+      </c>
       <c r="F18">
         <v>57129700</v>
       </c>
-      <c r="H18" s="4"/>
+      <c r="G18">
+        <v>44123700</v>
+      </c>
+      <c r="H18" s="4">
+        <f t="shared" ref="H18:H19" si="4">G18-F18</f>
+        <v>-13006000</v>
+      </c>
+      <c r="I18" s="8">
+        <f t="shared" ref="I18:I19" si="5">(H18)/F$11</f>
+        <v>-0.22765741812052226</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B19" s="4">
         <v>64011700</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="C19">
+        <v>66900400</v>
+      </c>
+      <c r="D19" s="4">
+        <f>C19-B19</f>
+        <v>2888700</v>
+      </c>
+      <c r="E19" s="8">
+        <f>(D19)/B$11</f>
+        <v>4.512768759461161E-2</v>
+      </c>
       <c r="F19">
         <v>57129700</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="G19" s="4">
+        <v>46238000</v>
+      </c>
+      <c r="H19" s="4">
+        <f>G19-F19</f>
+        <v>-10891700</v>
+      </c>
+      <c r="I19" s="8">
+        <f t="shared" si="5"/>
+        <v>-0.19064864685093744</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B20" s="4">
         <v>64011700</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="C20" s="4">
+        <v>111095000</v>
+      </c>
+      <c r="D20" s="4">
+        <f>C20-B20</f>
+        <v>47083300</v>
+      </c>
+      <c r="E20" s="8">
+        <f t="shared" ref="E20:E22" si="6">(D20)/B$11</f>
+        <v>0.73554209621053657</v>
+      </c>
       <c r="F20">
         <v>57129700</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="G20" s="4">
+        <v>91717700</v>
+      </c>
+      <c r="H20" s="4">
+        <f t="shared" ref="H20:H22" si="7">G20-F20</f>
+        <v>34588000</v>
+      </c>
+      <c r="I20" s="8">
+        <f t="shared" ref="I20:I22" si="8">(H20)/F$11</f>
+        <v>0.60542940011937751</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4">
         <v>64011700</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="C21" s="4">
+        <v>114667000</v>
+      </c>
+      <c r="D21" s="4">
+        <f>C21-B21</f>
+        <v>50655300</v>
+      </c>
+      <c r="E21" s="8">
+        <f t="shared" si="6"/>
+        <v>0.79134439485281594</v>
+      </c>
       <c r="F21">
         <v>57129700</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="G21" s="4">
+        <v>95290300</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="7"/>
+        <v>38160600</v>
+      </c>
+      <c r="I21" s="8">
+        <f t="shared" si="8"/>
+        <v>0.66796429877979402</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4">
+        <v>64011700</v>
+      </c>
+      <c r="C22" s="4">
+        <v>114116000</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" ref="D22" si="9">C22-B22</f>
+        <v>50104300</v>
+      </c>
+      <c r="E22" s="8">
+        <f t="shared" si="6"/>
+        <v>0.78273659346650692</v>
+      </c>
+      <c r="F22">
+        <v>57129700</v>
+      </c>
+      <c r="G22" s="4">
+        <v>94767200</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" si="7"/>
+        <v>37637500</v>
+      </c>
+      <c r="I22" s="8">
+        <f t="shared" si="8"/>
+        <v>0.6588079405283066</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
@@ -928,6 +1036,16 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Completed update of Unit Tests and tested from App install Change to handling of 'All' volumes (see manual) meant that all TestData files had to be updated. Yangtze 30EM would not run. Qtp arrays changed size. Not sure if this is a problem but it was resolved by changing the array check in graph2matrix.m at line 82.
git-svn-id: svn://192.168.0.80/muiApps/Trunk/Asmita@169 5305ae0c-0cd9-424f-b575-fb45b188e99a
</commit_message>
<xml_diff>
--- a/Training exercise/Training exercise-Southampton/SW4e_results.xlsx
+++ b/Training exercise/Training exercise-Southampton/SW4e_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab Code\MUImodels\muiApps\Asmita\Training exercise\Training exercise-Southampton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD063B08-DD0C-474B-A772-5ABD9DFD22E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047EF121-6672-4328-A08D-1B58E1C20F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13950" yWindow="6640" windowWidth="21940" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10480" yWindow="2500" windowWidth="21940" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -505,7 +505,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -899,32 +899,32 @@
         <v>11</v>
       </c>
       <c r="B19" s="4">
-        <v>64011700</v>
+        <v>65320700</v>
       </c>
       <c r="C19" s="4">
         <v>66900400</v>
       </c>
       <c r="D19" s="4">
         <f>C19-B19</f>
-        <v>2888700</v>
+        <v>1579700</v>
       </c>
       <c r="E19" s="8">
         <f>(D19)/B$11</f>
-        <v>4.512768759461161E-2</v>
+        <v>2.4678300998098784E-2</v>
       </c>
       <c r="F19" s="4">
-        <v>57129700</v>
+        <v>59209900</v>
       </c>
       <c r="G19" s="4">
         <v>46238000</v>
       </c>
       <c r="H19" s="4">
         <f>G19-F19</f>
-        <v>-10891700</v>
+        <v>-12971900</v>
       </c>
       <c r="I19" s="8">
         <f t="shared" si="5"/>
-        <v>-0.19064864685093744</v>
+        <v>-0.22706053068719073</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>